<commit_message>
ajuste de iconos listado de presentaciones
</commit_message>
<xml_diff>
--- a/assets/docs/Formato programacion.xlsx
+++ b/assets/docs/Formato programacion.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="57">
   <si>
     <t>Formato programacion</t>
   </si>
@@ -183,6 +183,9 @@
   </si>
   <si>
     <t>VERDURAS</t>
+  </si>
+  <si>
+    <t>CUARTO CICLO</t>
   </si>
 </sst>
 </file>
@@ -606,10 +609,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:P21"/>
+  <dimension ref="A1:P32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="P21" sqref="P21"/>
+      <selection activeCell="P32" sqref="P32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1424,6 +1427,458 @@
       <c r="O21" s="3"/>
       <c r="P21" s="3"/>
     </row>
+    <row r="22" spans="1:16">
+      <c r="A22" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F22" s="3">
+        <v>100</v>
+      </c>
+      <c r="G22" s="3">
+        <v>1</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I22" s="3">
+        <v>2</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="O22" s="3"/>
+      <c r="P22" s="3"/>
+    </row>
+    <row r="23" spans="1:16">
+      <c r="A23" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F23" s="3">
+        <v>100</v>
+      </c>
+      <c r="G23" s="3">
+        <v>1</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I23" s="3">
+        <v>2</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L23" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="M23" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N23" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="O23" s="3">
+        <v>100</v>
+      </c>
+      <c r="P23" s="3">
+        <v>7.75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
+      <c r="A24" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F24" s="3">
+        <v>100</v>
+      </c>
+      <c r="G24" s="3">
+        <v>1</v>
+      </c>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="3"/>
+    </row>
+    <row r="25" spans="1:16">
+      <c r="A25" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F25" s="3">
+        <v>100</v>
+      </c>
+      <c r="G25" s="3">
+        <v>1</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I25" s="3">
+        <v>2</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="K25" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="M25" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="N25" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="O25" s="3">
+        <v>100</v>
+      </c>
+      <c r="P25" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
+      <c r="A26" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F26" s="3">
+        <v>100</v>
+      </c>
+      <c r="G26" s="3">
+        <v>1</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I26" s="3">
+        <v>21</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L26" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="M26" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N26" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="O26" s="3">
+        <v>100</v>
+      </c>
+      <c r="P26" s="3">
+        <v>7.75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
+      <c r="A27" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F27" s="3">
+        <v>100</v>
+      </c>
+      <c r="G27" s="3">
+        <v>1</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I27" s="3">
+        <v>43</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="O27" s="3"/>
+      <c r="P27" s="3"/>
+    </row>
+    <row r="28" spans="1:16">
+      <c r="A28" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F28" s="3">
+        <v>100</v>
+      </c>
+      <c r="G28" s="3">
+        <v>1</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I28" s="3">
+        <v>4</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="O28" s="3"/>
+      <c r="P28" s="3"/>
+    </row>
+    <row r="29" spans="1:16">
+      <c r="A29" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F29" s="3">
+        <v>100</v>
+      </c>
+      <c r="G29" s="3">
+        <v>1</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I29" s="3">
+        <v>1</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="O29" s="3"/>
+      <c r="P29" s="3"/>
+    </row>
+    <row r="30" spans="1:16">
+      <c r="A30" s="3"/>
+      <c r="B30" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="3"/>
+      <c r="O30" s="3"/>
+      <c r="P30" s="3"/>
+    </row>
+    <row r="31" spans="1:16">
+      <c r="A31" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F31" s="3">
+        <v>100</v>
+      </c>
+      <c r="G31" s="3">
+        <v>1</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I31" s="3">
+        <v>2</v>
+      </c>
+      <c r="J31" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="O31" s="3"/>
+      <c r="P31" s="3"/>
+    </row>
+    <row r="32" spans="1:16">
+      <c r="A32" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F32" s="3">
+        <v>100</v>
+      </c>
+      <c r="G32" s="3">
+        <v>1</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I32" s="3">
+        <v>2</v>
+      </c>
+      <c r="J32" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K32" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L32" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="M32" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N32" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="O32" s="3">
+        <v>100</v>
+      </c>
+      <c r="P32" s="3">
+        <v>7.75</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <printOptions gridLines="false" gridLinesSet="true"/>

</xml_diff>